<commit_message>
Code for Jove Publication
Code for Published Jove Manuscript
</commit_message>
<xml_diff>
--- a/FileName.xlsx
+++ b/FileName.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msolufse/Dropbox/JovePaper/ValsalvaAnalyzer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msolufse/Documents/GitHub/ValsalvaAnalyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE48373-63EE-0945-BB46-4CC9F7DDFC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DFEF27-AC01-6940-885B-B76A77BD1B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,38 +20,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+  <si>
+    <t>m</t>
+  </si>
   <si>
     <t>Patient</t>
   </si>
   <si>
-    <t>Subject_1</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
-    <t>35</t>
-  </si>
-  <si>
     <t>Sex</t>
   </si>
   <si>
-    <t>m</t>
-  </si>
-  <si>
     <t>Height</t>
   </si>
   <si>
-    <t>176</t>
-  </si>
-  <si>
     <t>Weight</t>
   </si>
   <si>
-    <t>92</t>
-  </si>
-  <si>
     <t>T_1</t>
   </si>
   <si>
@@ -109,7 +97,13 @@
     <t>HR4_min</t>
   </si>
   <si>
-    <t>VR</t>
+    <t>HR_Max</t>
+  </si>
+  <si>
+    <t>VR1</t>
+  </si>
+  <si>
+    <t>VR2</t>
   </si>
   <si>
     <t>RRb_mean</t>
@@ -136,34 +130,67 @@
     <t>BRSv2eHRTD</t>
   </si>
   <si>
+    <t>R2_BRSv2eHRTD</t>
+  </si>
+  <si>
     <t>BRSv2eRRTD</t>
   </si>
   <si>
+    <t>R2_BRSv2eRRTD</t>
+  </si>
+  <si>
     <t>BRSv2eSPTD</t>
   </si>
   <si>
+    <t>R2_BRSv2eSPTD</t>
+  </si>
+  <si>
     <t>BRSv2eHRSP</t>
   </si>
   <si>
+    <t>R2_BRSv2eHRSP</t>
+  </si>
+  <si>
     <t>BRSv2eRRSP</t>
   </si>
   <si>
+    <t>R2_BRSv2eRRSP</t>
+  </si>
+  <si>
     <t>BRSa2lSPTD</t>
   </si>
   <si>
+    <t>R2_BRSa2lSPTD</t>
+  </si>
+  <si>
     <t>BRSv4eHRTD</t>
   </si>
   <si>
+    <t>R2_BRSv4eHRTD</t>
+  </si>
+  <si>
     <t>BRSv4eRRTD</t>
   </si>
   <si>
+    <t>R2_BRSv4eRRTD</t>
+  </si>
+  <si>
     <t>BRSv4eSPTD</t>
   </si>
   <si>
+    <t>R2_BRSv4eSPTD</t>
+  </si>
+  <si>
     <t>BRSv4eHRSP</t>
   </si>
   <si>
+    <t>R2_BRSv4eHRSP</t>
+  </si>
+  <si>
     <t>BRSv4eRRSP</t>
+  </si>
+  <si>
+    <t>R2_BRSv4eRRSP</t>
   </si>
   <si>
     <t>A</t>
@@ -248,10 +275,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -274,8 +306,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,15 +643,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BQ2"/>
+  <dimension ref="A1:CD2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
     <col min="2" max="2" width="4.5" customWidth="1"/>
     <col min="3" max="3" width="4.33203125" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
@@ -628,270 +661,353 @@
     <col min="8" max="8" width="4.6640625" customWidth="1"/>
     <col min="9" max="9" width="4.1640625" customWidth="1"/>
     <col min="10" max="10" width="6.5" customWidth="1"/>
-    <col min="11" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="32" width="12.6640625" customWidth="1"/>
-    <col min="33" max="33" width="12.33203125" customWidth="1"/>
-    <col min="34" max="35" width="12.5" customWidth="1"/>
-    <col min="36" max="36" width="13.5" customWidth="1"/>
-    <col min="37" max="37" width="12" customWidth="1"/>
-    <col min="38" max="39" width="12.5" customWidth="1"/>
-    <col min="40" max="40" width="12.6640625" customWidth="1"/>
-    <col min="41" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
+    <col min="13" max="13" width="9.83203125" customWidth="1"/>
+    <col min="14" max="14" width="9.5" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" customWidth="1"/>
+    <col min="19" max="19" width="10.5" customWidth="1"/>
+    <col min="20" max="21" width="10.1640625" customWidth="1"/>
+    <col min="22" max="22" width="10.5" customWidth="1"/>
+    <col min="23" max="23" width="10.1640625" customWidth="1"/>
+    <col min="24" max="24" width="9" customWidth="1"/>
+    <col min="25" max="25" width="8.33203125" customWidth="1"/>
+    <col min="26" max="27" width="4.5" customWidth="1"/>
+    <col min="28" max="29" width="10.5" customWidth="1"/>
+    <col min="30" max="30" width="10.33203125" customWidth="1"/>
+    <col min="31" max="32" width="10" customWidth="1"/>
+    <col min="33" max="33" width="10.33203125" customWidth="1"/>
+    <col min="34" max="34" width="9.1640625" customWidth="1"/>
+    <col min="35" max="35" width="12.33203125" customWidth="1"/>
+    <col min="36" max="36" width="15.5" customWidth="1"/>
+    <col min="37" max="37" width="12.1640625" customWidth="1"/>
+    <col min="38" max="38" width="15.33203125" customWidth="1"/>
+    <col min="39" max="39" width="12" customWidth="1"/>
+    <col min="40" max="40" width="15.1640625" customWidth="1"/>
+    <col min="41" max="41" width="12.1640625" customWidth="1"/>
+    <col min="42" max="42" width="15.33203125" customWidth="1"/>
     <col min="43" max="43" width="12" customWidth="1"/>
-    <col min="44" max="46" width="12.5" customWidth="1"/>
-    <col min="47" max="47" width="11.6640625" customWidth="1"/>
-    <col min="48" max="48" width="12.5" customWidth="1"/>
-    <col min="49" max="49" width="12.6640625" customWidth="1"/>
-    <col min="50" max="50" width="11.6640625" customWidth="1"/>
-    <col min="51" max="51" width="12.6640625" customWidth="1"/>
-    <col min="52" max="52" width="11.6640625" customWidth="1"/>
-    <col min="53" max="53" width="12.5" customWidth="1"/>
-    <col min="54" max="55" width="11.6640625" customWidth="1"/>
-    <col min="56" max="56" width="12.6640625" customWidth="1"/>
-    <col min="57" max="57" width="12.5" customWidth="1"/>
-    <col min="58" max="59" width="14.6640625" customWidth="1"/>
-    <col min="60" max="60" width="11.6640625" customWidth="1"/>
-    <col min="61" max="63" width="12.6640625" customWidth="1"/>
-    <col min="64" max="64" width="11.6640625" customWidth="1"/>
-    <col min="65" max="65" width="13.6640625" customWidth="1"/>
-    <col min="66" max="66" width="12.6640625" customWidth="1"/>
-    <col min="67" max="69" width="11.6640625" customWidth="1"/>
+    <col min="44" max="44" width="15.1640625" customWidth="1"/>
+    <col min="45" max="45" width="11.5" customWidth="1"/>
+    <col min="46" max="46" width="14.5" customWidth="1"/>
+    <col min="47" max="47" width="12.33203125" customWidth="1"/>
+    <col min="48" max="48" width="15.5" customWidth="1"/>
+    <col min="49" max="49" width="12.1640625" customWidth="1"/>
+    <col min="50" max="50" width="15.33203125" customWidth="1"/>
+    <col min="51" max="51" width="12" customWidth="1"/>
+    <col min="52" max="52" width="15.1640625" customWidth="1"/>
+    <col min="53" max="53" width="12.1640625" customWidth="1"/>
+    <col min="54" max="54" width="15.33203125" customWidth="1"/>
+    <col min="55" max="55" width="12" customWidth="1"/>
+    <col min="56" max="56" width="15.1640625" customWidth="1"/>
+    <col min="57" max="57" width="2.5" customWidth="1"/>
+    <col min="58" max="59" width="2.33203125" customWidth="1"/>
+    <col min="60" max="60" width="2.5" customWidth="1"/>
+    <col min="61" max="61" width="2.1640625" customWidth="1"/>
+    <col min="62" max="62" width="5.5" customWidth="1"/>
+    <col min="63" max="63" width="6.5" customWidth="1"/>
+    <col min="64" max="64" width="11.33203125" customWidth="1"/>
+    <col min="65" max="65" width="10.5" customWidth="1"/>
+    <col min="66" max="66" width="6" customWidth="1"/>
+    <col min="67" max="67" width="5.1640625" customWidth="1"/>
+    <col min="68" max="68" width="11.1640625" customWidth="1"/>
+    <col min="69" max="69" width="10.33203125" customWidth="1"/>
+    <col min="70" max="70" width="10.5" customWidth="1"/>
+    <col min="71" max="71" width="5.5" customWidth="1"/>
+    <col min="72" max="72" width="6.5" customWidth="1"/>
+    <col min="73" max="73" width="5.33203125" customWidth="1"/>
+    <col min="74" max="74" width="4.83203125" customWidth="1"/>
+    <col min="75" max="76" width="4.5" customWidth="1"/>
+    <col min="77" max="77" width="4" customWidth="1"/>
+    <col min="78" max="78" width="4.5" customWidth="1"/>
+    <col min="79" max="79" width="4.1640625" customWidth="1"/>
+    <col min="80" max="80" width="4.33203125" customWidth="1"/>
+    <col min="81" max="81" width="4" customWidth="1"/>
+    <col min="82" max="82" width="5.5" customWidth="1"/>
+    <col min="83" max="83" width="4.5" customWidth="1"/>
+    <col min="84" max="84" width="4" customWidth="1"/>
+    <col min="85" max="85" width="4.5" customWidth="1"/>
+    <col min="86" max="86" width="4.1640625" customWidth="1"/>
+    <col min="87" max="87" width="4.33203125" customWidth="1"/>
+    <col min="88" max="88" width="4" customWidth="1"/>
+    <col min="89" max="89" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>22</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>23</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>24</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Y1" t="s">
         <v>25</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
         <v>26</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AA1" t="s">
         <v>27</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AB1" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AD1" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AE1" t="s">
         <v>31</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AF1" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AG1" t="s">
         <v>33</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AH1" t="s">
         <v>34</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AI1" t="s">
         <v>35</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AJ1" t="s">
         <v>36</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AK1" t="s">
         <v>37</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AL1" t="s">
         <v>38</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AM1" t="s">
         <v>39</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AN1" t="s">
         <v>40</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AO1" t="s">
         <v>41</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AP1" t="s">
         <v>42</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AQ1" t="s">
         <v>43</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AR1" t="s">
         <v>44</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AS1" t="s">
         <v>45</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AT1" t="s">
         <v>46</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AU1" t="s">
         <v>47</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AV1" t="s">
         <v>48</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AW1" t="s">
         <v>49</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AX1" t="s">
         <v>50</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AY1" t="s">
         <v>51</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AZ1" t="s">
         <v>52</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BA1" t="s">
         <v>53</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BB1" t="s">
         <v>54</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BC1" t="s">
         <v>55</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BD1" t="s">
         <v>56</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BE1" t="s">
         <v>57</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BF1" t="s">
         <v>58</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BG1" t="s">
         <v>59</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BH1" t="s">
         <v>60</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BI1" t="s">
         <v>61</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BJ1" t="s">
         <v>62</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BK1" t="s">
         <v>63</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BL1" t="s">
         <v>64</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BM1" t="s">
         <v>65</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BN1" t="s">
         <v>66</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BO1" t="s">
         <v>67</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BP1" t="s">
         <v>68</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BQ1" t="s">
         <v>69</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BR1" t="s">
         <v>70</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BS1" t="s">
         <v>71</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BT1" t="s">
         <v>72</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BU1" t="s">
         <v>73</v>
       </c>
+      <c r="BV1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="2" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+      <c r="B2">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>176</v>
+      </c>
+      <c r="E2">
+        <v>92</v>
       </c>
       <c r="F2">
-        <v>2.8000000000000007</v>
+        <v>2.6000000000000014</v>
       </c>
       <c r="G2">
-        <v>5.1999999999999993</v>
+        <v>5.1999999999999975</v>
       </c>
       <c r="H2">
-        <v>11.3</v>
+        <v>11.300000000000004</v>
       </c>
       <c r="I2">
         <v>1.2999999999999972</v>
@@ -900,181 +1016,220 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>105.52707746891431</v>
+        <v>106.17345476232337</v>
       </c>
       <c r="L2">
-        <v>119.50913024322662</v>
+        <v>119.76829520812441</v>
       </c>
       <c r="M2">
-        <v>68.447382108982083</v>
+        <v>68.433783933674249</v>
       </c>
       <c r="N2">
-        <v>99.788741949209069</v>
+        <v>99.785555523046796</v>
       </c>
       <c r="O2">
-        <v>99.388518046619112</v>
+        <v>99.284195040118391</v>
       </c>
       <c r="P2">
-        <v>74.190524817701004</v>
+        <v>74.178824909778541</v>
       </c>
       <c r="Q2">
-        <v>140.60975609756099</v>
+        <v>140.60975609756096</v>
       </c>
       <c r="R2">
-        <v>90.168969883094732</v>
+        <v>87.96411891723038</v>
       </c>
       <c r="S2">
-        <v>52.114222165094155</v>
+        <v>51.356340615340521</v>
       </c>
       <c r="T2">
-        <v>74.098598433568597</v>
+        <v>74.140327865838699</v>
       </c>
       <c r="U2">
-        <v>104.48093824955566</v>
+        <v>104.54262063419709</v>
       </c>
       <c r="V2">
-        <v>133.208041958042</v>
+        <v>134.67657342657344</v>
       </c>
       <c r="W2">
-        <v>68.59265734265739</v>
+        <v>68.592657342657361</v>
       </c>
       <c r="X2">
-        <v>40.789622025319133</v>
+        <v>40.788579197824703</v>
       </c>
       <c r="Y2">
-        <v>3.2657336681216722</v>
+        <v>134.52435061989851</v>
       </c>
       <c r="Z2">
-        <v>0.66541738336138023</v>
+        <v>3.3018206585081513</v>
       </c>
       <c r="AA2">
-        <v>1.1513171934126591</v>
+        <v>3.2980886626978378</v>
       </c>
       <c r="AB2">
-        <v>0.80973191488623941</v>
+        <v>0.68209629947475348</v>
       </c>
       <c r="AC2">
-        <v>0.57426743102831168</v>
+        <v>1.1683075406287331</v>
       </c>
       <c r="AD2">
-        <v>0.45042325611916778</v>
+        <v>809.27616220653272</v>
       </c>
       <c r="AE2">
-        <v>0.87472919587103293</v>
+        <v>573.92860094778712</v>
       </c>
       <c r="AF2">
-        <v>1.4709623924133572</v>
+        <v>445.51178035957679</v>
       </c>
       <c r="AG2">
-        <v>6.2456373356999464</v>
+        <v>874.72919587103331</v>
       </c>
       <c r="AH2">
-        <v>-48.538574440008759</v>
+        <v>1470.9999999999966</v>
       </c>
       <c r="AI2">
-        <v>-10.226466879762112</v>
+        <v>6.2491899886815476</v>
       </c>
       <c r="AJ2">
-        <v>-0.55748110941572981</v>
+        <v>0.99670035961287151</v>
       </c>
       <c r="AK2">
-        <v>4.4514758022358523</v>
+        <v>-48.490762596464826</v>
       </c>
       <c r="AL2">
-        <v>3.3107385319844767</v>
+        <v>0.98899643535971915</v>
       </c>
       <c r="AM2">
-        <v>-65.555999859736886</v>
+        <v>-10.183422893894138</v>
       </c>
       <c r="AN2">
-        <v>0.36024864257960565</v>
+        <v>0.91126954647069136</v>
       </c>
       <c r="AO2">
-        <v>24.698634986456103</v>
+        <v>-0.55910811347111355</v>
       </c>
       <c r="AP2">
-        <v>-2.9890575667786714</v>
+        <v>0.9079239014293693</v>
       </c>
       <c r="AQ2">
-        <v>16.463935908574555</v>
+        <v>4.4591120532952324</v>
       </c>
       <c r="AR2">
-        <v>-37.079695359932231</v>
+        <v>0.95173090383434988</v>
       </c>
       <c r="AS2">
-        <v>-25.197993228918108</v>
+        <v>3.3116017471065144</v>
       </c>
       <c r="AT2">
-        <v>30.941135937637029</v>
+        <v>0.98485773910417751</v>
       </c>
       <c r="AU2">
-        <v>31.33655265121331</v>
+        <v>-87.643001924327436</v>
       </c>
       <c r="AV2">
-        <v>35.082678628646676</v>
+        <v>0.92272272397380195</v>
       </c>
       <c r="AW2">
-        <v>25.197993228918108</v>
+        <v>511.12824459399485</v>
       </c>
       <c r="AX2">
-        <v>55.978190281620812</v>
+        <v>0.85508285118565008</v>
       </c>
       <c r="AY2">
-        <v>2.7381536227997367</v>
+        <v>25.67321372693884</v>
       </c>
       <c r="AZ2">
-        <v>31.33655265121331</v>
+        <v>0.98142924898858108</v>
       </c>
       <c r="BA2">
-        <v>73.193194510273543</v>
+        <v>-4.0557656914351696</v>
       </c>
       <c r="BB2">
-        <v>88.354159594592602</v>
+        <v>0.93192449338569505</v>
       </c>
       <c r="BC2">
-        <v>196.67442249253793</v>
+        <v>23.762742432444526</v>
       </c>
       <c r="BD2">
-        <v>17.401450150567257</v>
+        <v>0.87164539884357051</v>
       </c>
       <c r="BE2">
-        <v>3422.4201588955025</v>
+        <v>-37.739670828649125</v>
       </c>
       <c r="BF2">
-        <v>0.11216825712343181</v>
+        <v>-25.10537013033985</v>
       </c>
       <c r="BG2">
-        <v>0.24918555949158919</v>
+        <v>30.850411106444142</v>
       </c>
       <c r="BH2">
-        <v>88.814744119850488</v>
+        <v>31.994629852544833</v>
       </c>
       <c r="BI2">
-        <v>0.22007723716972294</v>
+        <v>34.436301335237587</v>
       </c>
       <c r="BJ2">
-        <v>0.22007723716972294</v>
+        <v>25.10537013033985</v>
       </c>
       <c r="BK2">
-        <v>0.22007723716972294</v>
+        <v>56.568698426404012</v>
       </c>
       <c r="BL2">
-        <v>78.470978506597774</v>
+        <v>2.7301248766764719</v>
       </c>
       <c r="BM2">
-        <v>0.23391405916286204</v>
+        <v>31.994629852544833</v>
       </c>
       <c r="BN2">
-        <v>0.325062665056431</v>
+        <v>73.197328513418512</v>
       </c>
       <c r="BO2">
-        <v>1.4437153242087521</v>
+        <v>88.363549648812253</v>
       </c>
       <c r="BP2">
-        <v>40.789622025319126</v>
+        <v>196.7257017868624</v>
       </c>
       <c r="BQ2">
-        <v>45.167425157438245</v>
+        <v>17.501355549123332</v>
+      </c>
+      <c r="BR2">
+        <v>3442.9664526226861</v>
+      </c>
+      <c r="BS2">
+        <v>0.11194765855063651</v>
+      </c>
+      <c r="BT2">
+        <v>0.25224616499240116</v>
+      </c>
+      <c r="BU2">
+        <v>89.685818894700844</v>
+      </c>
+      <c r="BV2">
+        <v>0.22021815695505173</v>
+      </c>
+      <c r="BW2">
+        <v>0.22021815695505173</v>
+      </c>
+      <c r="BX2">
+        <v>0.22021815695505173</v>
+      </c>
+      <c r="BY2">
+        <v>84.215887534985839</v>
+      </c>
+      <c r="BZ2">
+        <v>0.14916591371663834</v>
+      </c>
+      <c r="CA2">
+        <v>0.47057148769308954</v>
+      </c>
+      <c r="CB2">
+        <v>1.0888705489902537</v>
+      </c>
+      <c r="CC2">
+        <v>40.788579197824696</v>
+      </c>
+      <c r="CD2">
+        <v>34.177011558824567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>